<commit_message>
1. Upper Char SheetName/tableName 2. Change Default value case no Data to NULL 3. Support Default field STATUS_DT
</commit_message>
<xml_diff>
--- a/SQLInsertGenerator/book1.xlsx
+++ b/SQLInsertGenerator/book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://awarecorp-my.sharepoint.com/personal/theedanai_p_aware_co_th/Documents/Automate python/SQLInsertGenerator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://awarecorp-my.sharepoint.com/personal/theedanai_p_aware_co_th/Documents/Automate-python/SQLInsertGenerator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:40009_{57132196-05A3-48F3-A834-6A38357E734C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4801D4F1-9DBA-4BEA-BC3A-A6B250A68C9B}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:40009_{57132196-05A3-48F3-A834-6A38357E734C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B15967B-D6AD-433E-8C4F-C5BAAD4809D1}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="31620" yWindow="4965" windowWidth="25785" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sff_cfg_lov" sheetId="1" r:id="rId1"/>
@@ -499,8 +499,8 @@
   </sheetPr>
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -518,8 +518,8 @@
     <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
     <col min="14" max="14" width="20.140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="20.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="23.7109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="25.42578125" style="1" customWidth="1"/>
     <col min="18" max="18" width="15.42578125" style="2" customWidth="1"/>
     <col min="19" max="19" width="15.140625" style="2" customWidth="1"/>
     <col min="20" max="20" width="18.5703125" style="2" customWidth="1"/>
@@ -638,9 +638,13 @@
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
-      <c r="O2" s="7"/>
+      <c r="O2" s="7">
+        <v>44843.016400462962</v>
+      </c>
       <c r="P2" s="6"/>
-      <c r="Q2" s="7"/>
+      <c r="Q2" s="7">
+        <v>44843.016400462962</v>
+      </c>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6" t="s">
@@ -696,9 +700,13 @@
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
-      <c r="O3" s="7"/>
+      <c r="O3" s="7">
+        <v>44843.016400462962</v>
+      </c>
       <c r="P3" s="6"/>
-      <c r="Q3" s="7"/>
+      <c r="Q3" s="7">
+        <v>44843.016400462962</v>
+      </c>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6" t="s">
@@ -754,9 +762,13 @@
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
-      <c r="O4" s="7"/>
+      <c r="O4" s="7">
+        <v>44843.016400462962</v>
+      </c>
       <c r="P4" s="6"/>
-      <c r="Q4" s="7"/>
+      <c r="Q4" s="7">
+        <v>44843.016400462962</v>
+      </c>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6" t="s">
@@ -1852,7 +1864,7 @@
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>